<commit_message>
Minor tweaks to the ruby squib generator
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -17,40 +17,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Subtitle</t>
-  </si>
-  <si>
-    <t>Frame</t>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>Warmup</t>
-  </si>
-  <si>
-    <t>Cooldown</t>
-  </si>
-  <si>
-    <t>Damage</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Creation Year</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>Description</t>
+    <t>title</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>warmup</t>
+  </si>
+  <si>
+    <t>cooldown</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>creation_year</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
   <si>
     <t>Dagger</t>
@@ -323,7 +323,7 @@
   <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>